<commit_message>
scripts aula 02 e 03
</commit_message>
<xml_diff>
--- a/misc/Caderneta-2022.xlsx
+++ b/misc/Caderneta-2022.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="38">
   <si>
     <t>RA</t>
   </si>
@@ -543,7 +543,7 @@
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -593,7 +593,7 @@
                   <a14:compatExt spid="_x0000_s1026"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -643,7 +643,7 @@
                   <a14:compatExt spid="_x0000_s1027"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -693,7 +693,7 @@
                   <a14:compatExt spid="_x0000_s1028"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -743,7 +743,7 @@
                   <a14:compatExt spid="_x0000_s1029"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -793,7 +793,7 @@
                   <a14:compatExt spid="_x0000_s1030"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -827,13 +827,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>185487</xdr:rowOff>
+          <xdr:rowOff>175962</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>169946</xdr:colOff>
-          <xdr:row>9</xdr:row>
-          <xdr:rowOff>1003</xdr:rowOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>212057</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -843,7 +843,7 @@
                   <a14:compatExt spid="_x0000_s1031"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -877,13 +877,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>184484</xdr:rowOff>
+          <xdr:rowOff>174959</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>169946</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>20053</xdr:rowOff>
+          <xdr:rowOff>10528</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -893,7 +893,7 @@
                   <a14:compatExt spid="_x0000_s1032"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1437,7 +1437,182 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId18" name="Control 1">
+        <control shapeId="1032" r:id="rId18" name="Control 8">
+          <controlPr defaultSize="0" r:id="rId19">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>171450</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1032" r:id="rId18" name="Control 8"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1031" r:id="rId20" name="Control 7">
+          <controlPr defaultSize="0" r:id="rId19">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>171450</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>209550</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1031" r:id="rId20" name="Control 7"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1030" r:id="rId21" name="Control 6">
+          <controlPr defaultSize="0" r:id="rId22">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>171450</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1030" r:id="rId21" name="Control 6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1029" r:id="rId23" name="Control 5">
+          <controlPr defaultSize="0" r:id="rId22">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>171450</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1029" r:id="rId23" name="Control 5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1028" r:id="rId24" name="Control 4">
+          <controlPr defaultSize="0" r:id="rId22">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>171450</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1028" r:id="rId24" name="Control 4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1027" r:id="rId25" name="Control 3">
+          <controlPr defaultSize="0" r:id="rId19">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>171450</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1027" r:id="rId25" name="Control 3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1026" r:id="rId26" name="Control 2">
+          <controlPr defaultSize="0" r:id="rId19">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>171450</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1026" r:id="rId26" name="Control 2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1025" r:id="rId27" name="Control 1">
           <controlPr defaultSize="0" r:id="rId19">
             <anchor moveWithCells="1">
               <from>
@@ -1457,182 +1632,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId18" name="Control 1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId20" name="Control 2">
-          <controlPr defaultSize="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>171450</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1026" r:id="rId20" name="Control 2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1027" r:id="rId21" name="Control 3">
-          <controlPr defaultSize="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>171450</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1027" r:id="rId21" name="Control 3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1028" r:id="rId22" name="Control 4">
-          <controlPr defaultSize="0" r:id="rId23">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>171450</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1028" r:id="rId22" name="Control 4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1029" r:id="rId24" name="Control 5">
-          <controlPr defaultSize="0" r:id="rId23">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>171450</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1029" r:id="rId24" name="Control 5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1030" r:id="rId25" name="Control 6">
-          <controlPr defaultSize="0" r:id="rId23">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>171450</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1030" r:id="rId25" name="Control 6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1031" r:id="rId26" name="Control 7">
-          <controlPr defaultSize="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>171450</xdr:colOff>
-                <xdr:row>9</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1031" r:id="rId26" name="Control 7"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1032" r:id="rId27" name="Control 8">
-          <controlPr defaultSize="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>171450</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1032" r:id="rId27" name="Control 8"/>
+        <control shapeId="1025" r:id="rId27" name="Control 1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -1668,7 +1668,7 @@
   <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1751,7 +1751,9 @@
       <c r="D2" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="23"/>
+      <c r="E2" s="23" t="s">
+        <v>35</v>
+      </c>
       <c r="F2" s="23"/>
       <c r="G2" s="23"/>
       <c r="H2" s="23"/>
@@ -1780,7 +1782,9 @@
       <c r="D3" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="25"/>
+      <c r="E3" s="25" t="s">
+        <v>35</v>
+      </c>
       <c r="F3" s="25"/>
       <c r="G3" s="25"/>
       <c r="H3" s="25"/>
@@ -1809,7 +1813,9 @@
       <c r="D4" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="23"/>
+      <c r="E4" s="23" t="s">
+        <v>35</v>
+      </c>
       <c r="F4" s="23"/>
       <c r="G4" s="23"/>
       <c r="H4" s="23"/>
@@ -1838,7 +1844,9 @@
       <c r="D5" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="25"/>
+      <c r="E5" s="25" t="s">
+        <v>35</v>
+      </c>
       <c r="F5" s="25"/>
       <c r="G5" s="25"/>
       <c r="H5" s="25"/>
@@ -1867,7 +1875,9 @@
       <c r="D6" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="23"/>
+      <c r="E6" s="23" t="s">
+        <v>35</v>
+      </c>
       <c r="F6" s="23"/>
       <c r="G6" s="23"/>
       <c r="H6" s="23"/>
@@ -1896,7 +1906,9 @@
       <c r="D7" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="25"/>
+      <c r="E7" s="25" t="s">
+        <v>35</v>
+      </c>
       <c r="F7" s="25"/>
       <c r="G7" s="25"/>
       <c r="H7" s="25"/>
@@ -1925,7 +1937,9 @@
       <c r="D8" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="23"/>
+      <c r="E8" s="23" t="s">
+        <v>35</v>
+      </c>
       <c r="F8" s="23"/>
       <c r="G8" s="23"/>
       <c r="H8" s="23"/>
@@ -1938,7 +1952,7 @@
       <c r="O8" s="24"/>
       <c r="P8" s="28">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="16.5" customHeight="1" thickBot="1">
@@ -1954,7 +1968,9 @@
       <c r="D9" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="25"/>
+      <c r="E9" s="25" t="s">
+        <v>36</v>
+      </c>
       <c r="F9" s="25"/>
       <c r="G9" s="25"/>
       <c r="H9" s="25"/>

</xml_diff>